<commit_message>
benerin tampilan dan print
</commit_message>
<xml_diff>
--- a/laporan/Laporan_Penjualan_Mingguan_-_30-06-2025_s-d_06-07-2025.xlsx
+++ b/laporan/Laporan_Penjualan_Mingguan_-_30-06-2025_s-d_06-07-2025.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>No</t>
   </si>
@@ -92,16 +92,37 @@
     <t>30/06/2025 17:30:39</t>
   </si>
   <si>
+    <t>Baterai ABC AA</t>
+  </si>
+  <si>
+    <t>Elektronik</t>
+  </si>
+  <si>
+    <t>01/07/2025 00:06:44</t>
+  </si>
+  <si>
+    <t>01/07/2025 00:26:44</t>
+  </si>
+  <si>
+    <t>01/07/2025 10:09:05</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>02/07/2025 23:28:07</t>
+  </si>
+  <si>
     <t>GRAND TOTAL</t>
   </si>
   <si>
-    <t>Total Transaksi: 7</t>
+    <t>Total Transaksi: 11</t>
   </si>
   <si>
     <t>Periode: Mingguan - 30/06/2025 s/d 06/07/2025</t>
   </si>
   <si>
-    <t>Dibuat pada: 30/06/2025 21:56:13</t>
+    <t>Dibuat pada: 02/07/2025 23:59:17</t>
   </si>
 </sst>
 </file>
@@ -164,7 +185,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -393,33 +414,137 @@
         <v>25</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="B11" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E11" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="F11" t="n" s="0">
+        <v>6000.0</v>
+      </c>
+      <c r="G11" t="n" s="0">
+        <v>6000.0</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
     <row r="12">
-      <c r="A12" t="s" s="3">
-        <v>26</v>
-      </c>
-      <c r="G12" t="n" s="3">
-        <v>178500.0</v>
+      <c r="A12" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="B12" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E12" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F12" t="n" s="0">
+        <v>3500.0</v>
+      </c>
+      <c r="G12" t="n" s="0">
+        <v>17500.0</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B13" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E13" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="F13" t="n" s="0">
+        <v>20000.0</v>
+      </c>
+      <c r="G13" t="n" s="0">
+        <v>20000.0</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>30</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="0">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
-        <v>28</v>
+      <c r="A14" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="B14" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="E14" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="F14" t="n" s="0">
+        <v>1111.0</v>
+      </c>
+      <c r="G14" t="n" s="0">
+        <v>1111.0</v>
+      </c>
+      <c r="H14" t="s" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s" s="0">
-        <v>29</v>
+      <c r="A16" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="G16" t="n" s="3">
+        <v>223111.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A16:F16"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>